<commit_message>
Update MODELO 4.16 Integrado_Exportaciones_mensual.xlsx
</commit_message>
<xml_diff>
--- a/Agricultura/MODELOS/MODELO 4.16 Integrado_Exportaciones_mensual.xlsx
+++ b/Agricultura/MODELOS/MODELO 4.16 Integrado_Exportaciones_mensual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\DATA INTELLIGENCE Dropbox\Diseño DATA's\Tablas Madre\Agricultura\MODELOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E6D91A-789E-4C91-9A44-B8D9E6A475E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C3B19A-EB87-4414-9964-4971CE6BEC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{5402BD67-523E-46F2-97D3-E3B02C663DDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5402BD67-523E-46F2-97D3-E3B02C663DDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3561" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3678" uniqueCount="1116">
   <si>
     <t>2019/2020</t>
   </si>
@@ -3052,6 +3052,402 @@
   </si>
   <si>
     <t>https://analytics.zoho.com/open-view/2395394000011166773?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011642412?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011642823?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011642959?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011677005?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011677495?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011677639?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011677936?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011683306?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011683604?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011684065</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011684432</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011684587</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011684674?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011684744?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011684814?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011694141?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011694181?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011694221?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011694844?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011694880?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011694916?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011700394?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011700430?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011700466?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011700869?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011700916?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011700963?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011704681?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011704730?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011704779?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011707836?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011707886?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011707936?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011707986?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011709036?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011709086?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>CULTIVO</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011714436?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011766202?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011766298?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tipo (Orgánico/No orgánico) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- CULTIVO</t>
+    </r>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011766505?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011766716?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011766910?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011767471?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011768092?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011768282?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Procesamiento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- CULTIVO</t>
+    </r>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011712177?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011712445?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011712539?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011712699?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011770302?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011770486?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>GR 019</t>
+  </si>
+  <si>
+    <t>GR 020</t>
+  </si>
+  <si>
+    <t>GR 021</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011696442?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011696894?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011771224?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011771393?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011771544?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011771695?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001%0A</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774239?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774436?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774483?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774239</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774436</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774483</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774833?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774889?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011774945?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011775965?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777015?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777065?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777115?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777158?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777201?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777244?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777287?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777326?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777868?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777911?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011777959?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011778007?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011778064?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011778127?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011778190?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011778243?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011778296?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787034</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787067</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787797?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787837?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787877?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787917?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787953?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011787989?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011789569?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011789605?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011789641?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Categor%C3%ADa%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011789677?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011789724?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011789771?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011791342?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011791392?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011791442?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011791492?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011791542?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011791592?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_cultivo%22%3D100101001</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011796447?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Procesamiento%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011796821?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Procesamiento%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011797006?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Procesamiento%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011797134?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Procesamiento%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011797397?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Procesamiento%22%3D1</t>
+  </si>
+  <si>
+    <t>https://analytics.zoho.com/open-view/2395394000011797539?ZOHO_CRITERIA=%22Traspuesta%204.16_Mes%2FA%C3%B1o%22.%22Cod_Procesamiento%22%3D1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tipo (Orgánico/No orgánico) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- MES</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3061,7 +3457,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3214,8 +3610,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3273,6 +3683,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3349,7 +3777,7 @@
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3547,6 +3975,20 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -3554,6 +3996,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -3790,16 +4242,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4106,7 +4548,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>621753</xdr:colOff>
+      <xdr:colOff>440778</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -4178,13 +4620,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>870614</xdr:colOff>
+      <xdr:colOff>689639</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>804789</xdr:colOff>
+      <xdr:colOff>623814</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
@@ -4334,13 +4776,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>842889</xdr:colOff>
+      <xdr:colOff>661914</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>15241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>199035</xdr:colOff>
+      <xdr:colOff>18060</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
@@ -4412,13 +4854,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>276894</xdr:colOff>
+      <xdr:colOff>95919</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>30481</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>2011855</xdr:colOff>
+      <xdr:colOff>1830880</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
@@ -9147,14 +9589,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4CA779AC-3E97-4459-BF90-94F12FD2CEB9}" name="Cod_categoría" displayName="Cod_categoría" ref="B2:C111" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4CA779AC-3E97-4459-BF90-94F12FD2CEB9}" name="Cod_categoría" displayName="Cod_categoría" ref="B2:C111" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="B2:C111" xr:uid="{4CA779AC-3E97-4459-BF90-94F12FD2CEB9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C115">
     <sortCondition ref="B2:B115"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00A0CACF-8DA8-4EE1-B69E-D20C0D0CED17}" name="Cultivo" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{EC636045-613B-42E5-9C90-E988441BFFD8}" name="Id_Cultivo" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00A0CACF-8DA8-4EE1-B69E-D20C0D0CED17}" name="Cultivo" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{EC636045-613B-42E5-9C90-E988441BFFD8}" name="Id_Cultivo" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9177,36 +9619,36 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EC5FE2C8-06DB-4106-9461-CA393495CC9E}" name="Cod_procesamiento10" displayName="Cod_procesamiento10" ref="B2:C15" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EC5FE2C8-06DB-4106-9461-CA393495CC9E}" name="Cod_procesamiento10" displayName="Cod_procesamiento10" ref="B2:C15" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B2:C15" xr:uid="{EC5FE2C8-06DB-4106-9461-CA393495CC9E}"/>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{DFB3BE9C-F8B5-4C1F-822D-968586718286}" name="Tipo de cultivo" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{A7D9713B-9CA4-4D1C-8E9D-992303A697CD}" name="Id_Categoría" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{DFB3BE9C-F8B5-4C1F-822D-968586718286}" name="Tipo de cultivo" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{A7D9713B-9CA4-4D1C-8E9D-992303A697CD}" name="Id_Categoría" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{228B48F0-A424-4478-A649-00994AC4E152}" name="Cod_procesamiento" displayName="Cod_procesamiento" ref="B2:C8" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{228B48F0-A424-4478-A649-00994AC4E152}" name="Cod_procesamiento" displayName="Cod_procesamiento" ref="B2:C8" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="B2:C8" xr:uid="{228B48F0-A424-4478-A649-00994AC4E152}"/>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{EE422AE0-5FF5-4FF7-873B-6BC93A7C476F}" name="Procesamiento" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{775A3C91-EDE1-40BA-A829-E5FE120F9D39}" name="Id_Procesamiento" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{EE422AE0-5FF5-4FF7-873B-6BC93A7C476F}" name="Procesamiento" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{775A3C91-EDE1-40BA-A829-E5FE120F9D39}" name="Id_Procesamiento" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9DEBE778-257A-4F77-B952-D29267D603FC}" name="Cod_país" displayName="Cod_país" ref="B2:C161" totalsRowShown="0" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9DEBE778-257A-4F77-B952-D29267D603FC}" name="Cod_país" displayName="Cod_país" ref="B2:C161" totalsRowShown="0" tableBorderDxfId="3">
   <autoFilter ref="B2:C161" xr:uid="{9DEBE778-257A-4F77-B952-D29267D603FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C161">
     <sortCondition ref="B3:B161"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{11154556-49A8-4584-BF27-62A0E30BE082}" name="País de Destino" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{08D23EDC-011A-480F-92F3-73D7B20C32A8}" name="Código_País" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{11154556-49A8-4584-BF27-62A0E30BE082}" name="País de Destino" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{08D23EDC-011A-480F-92F3-73D7B20C32A8}" name="Código_País" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9512,7 +9954,7 @@
   <dimension ref="A3:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9908,10 +10350,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79036886-1897-4BCD-BB4E-BCAD8551FFA8}">
   <dimension ref="B1:W147"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="S30" sqref="S30"/>
+      <selection pane="bottomLeft" activeCell="K147" sqref="K147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9926,7 +10368,7 @@
     <col min="8" max="8" width="5.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" customWidth="1"/>
     <col min="12" max="12" width="26.5703125" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
     <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -10117,7 +10559,7 @@
       <c r="N12" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O12" s="45" t="str">
+      <c r="O12" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en Kg de arándano por Cultivo</v>
       </c>
@@ -10165,7 +10607,7 @@
       <c r="N13" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O13" s="45" t="str">
+      <c r="O13" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD de arándano por Cultivo</v>
       </c>
@@ -10212,7 +10654,7 @@
       <c r="N14" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O14" s="45" t="str">
+      <c r="O14" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de arándano por Cultivo</v>
       </c>
@@ -10259,7 +10701,7 @@
       <c r="N15" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O15" s="45" t="str">
+      <c r="O15" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en Kg de berries por Cultivo</v>
       </c>
@@ -10306,7 +10748,7 @@
       <c r="N16" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O16" s="45" t="str">
+      <c r="O16" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD de berries por Cultivo</v>
       </c>
@@ -10353,7 +10795,7 @@
       <c r="N17" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="45" t="str">
+      <c r="O17" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de berries por Cultivo</v>
       </c>
@@ -10400,7 +10842,7 @@
       <c r="N18" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O18" s="45" t="str">
+      <c r="O18" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -10447,7 +10889,7 @@
       <c r="N19" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O19" s="45" t="str">
+      <c r="O19" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en USD de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -10494,7 +10936,7 @@
       <c r="N20" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O20" s="45" t="str">
+      <c r="O20" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -10541,7 +10983,7 @@
       <c r="N21" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O21" s="45" t="str">
+      <c r="O21" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en Kg de Berries por Cultivo y Procesamiento</v>
       </c>
@@ -10588,7 +11030,7 @@
       <c r="N22" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O22" s="45" t="str">
+      <c r="O22" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en USD de Berries por Cultivo y Procesamiento</v>
       </c>
@@ -10635,7 +11077,7 @@
       <c r="N23" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O23" s="45" t="str">
+      <c r="O23" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de Berries por Cultivo y Procesamiento</v>
       </c>
@@ -10682,7 +11124,7 @@
       <c r="N24" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O24" s="45" t="str">
+      <c r="O24" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en Kg de Berries por Cultivo y País de Destino</v>
       </c>
@@ -10729,7 +11171,7 @@
       <c r="N25" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O25" s="45" t="str">
+      <c r="O25" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en USD de Berries por Cultivo y País de Destino</v>
       </c>
@@ -10776,7 +11218,7 @@
       <c r="N26" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O26" s="45" t="str">
+      <c r="O26" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de Berries por Cultivo y País de Destino</v>
       </c>
@@ -10823,7 +11265,7 @@
       <c r="N27" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O27" s="45" t="str">
+      <c r="O27" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en Kg de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -10870,7 +11312,7 @@
       <c r="N28" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O28" s="45" t="str">
+      <c r="O28" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -10917,7 +11359,7 @@
       <c r="N29" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O29" s="45" t="str">
+      <c r="O29" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -10964,7 +11406,7 @@
       <c r="N30" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O30" s="45" t="str">
+      <c r="O30" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en Kg de arándano por Año</v>
       </c>
@@ -10975,7 +11417,9 @@
       <c r="R30" s="48">
         <v>110</v>
       </c>
-      <c r="S30" s="15"/>
+      <c r="S30" s="15" t="s">
+        <v>996</v>
+      </c>
       <c r="V30" t="s">
         <v>949</v>
       </c>
@@ -11012,7 +11456,7 @@
       <c r="N31" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O31" s="45" t="str">
+      <c r="O31" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD de arándano por Año</v>
       </c>
@@ -11023,7 +11467,9 @@
       <c r="R31" s="48">
         <v>110</v>
       </c>
-      <c r="S31" s="15"/>
+      <c r="S31" s="15" t="s">
+        <v>997</v>
+      </c>
       <c r="V31" t="s">
         <v>949</v>
       </c>
@@ -11060,7 +11506,7 @@
       <c r="N32" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O32" s="45" t="str">
+      <c r="O32" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de arándano por Año</v>
       </c>
@@ -11071,7 +11517,9 @@
       <c r="R32" s="48">
         <v>110</v>
       </c>
-      <c r="S32" s="15"/>
+      <c r="S32" s="15" t="s">
+        <v>998</v>
+      </c>
       <c r="V32" t="s">
         <v>949</v>
       </c>
@@ -11108,7 +11556,7 @@
       <c r="N33" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O33" s="45" t="str">
+      <c r="O33" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en Kg de arándano por Procesamiento</v>
       </c>
@@ -11119,7 +11567,9 @@
       <c r="R33" s="48">
         <v>110</v>
       </c>
-      <c r="S33" s="15"/>
+      <c r="S33" s="15" t="s">
+        <v>999</v>
+      </c>
       <c r="V33" t="s">
         <v>949</v>
       </c>
@@ -11156,7 +11606,7 @@
       <c r="N34" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O34" s="45" t="str">
+      <c r="O34" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD de arándano por Procesamiento</v>
       </c>
@@ -11167,7 +11617,9 @@
       <c r="R34" s="48">
         <v>110</v>
       </c>
-      <c r="S34" s="15"/>
+      <c r="S34" s="15" t="s">
+        <v>1000</v>
+      </c>
       <c r="V34" t="s">
         <v>949</v>
       </c>
@@ -11204,7 +11656,7 @@
       <c r="N35" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O35" s="45" t="str">
+      <c r="O35" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de arándano por Procesamiento</v>
       </c>
@@ -11215,7 +11667,9 @@
       <c r="R35" s="48">
         <v>110</v>
       </c>
-      <c r="S35" s="15"/>
+      <c r="S35" s="15" t="s">
+        <v>1001</v>
+      </c>
       <c r="V35" t="s">
         <v>949</v>
       </c>
@@ -11252,7 +11706,7 @@
       <c r="N36" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O36" s="45" t="str">
+      <c r="O36" s="79" t="str">
         <f>"Evolución mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en Kg de arándano por País de destino</v>
       </c>
@@ -11263,7 +11717,9 @@
       <c r="R36" s="48">
         <v>110</v>
       </c>
-      <c r="S36" s="15"/>
+      <c r="S36" s="15" t="s">
+        <v>1002</v>
+      </c>
       <c r="V36" t="s">
         <v>949</v>
       </c>
@@ -11300,7 +11756,7 @@
       <c r="N37" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O37" s="45" t="str">
+      <c r="O37" s="80" t="str">
         <f>"Evolución mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD de arándano por País de destino</v>
       </c>
@@ -11311,7 +11767,9 @@
       <c r="R37" s="48">
         <v>110</v>
       </c>
-      <c r="S37" s="15"/>
+      <c r="S37" s="15" t="s">
+        <v>1003</v>
+      </c>
       <c r="V37" t="s">
         <v>949</v>
       </c>
@@ -11348,7 +11806,7 @@
       <c r="N38" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O38" s="57" t="str">
+      <c r="O38" s="81" t="str">
         <f>"Evolución mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Evolución mensual de Exportaciones en USD/Kg de arándano por País de destino</v>
       </c>
@@ -11359,7 +11817,9 @@
       <c r="R38" s="60">
         <v>110</v>
       </c>
-      <c r="S38" s="15"/>
+      <c r="S38" s="15" t="s">
+        <v>1004</v>
+      </c>
       <c r="V38" t="s">
         <v>949</v>
       </c>
@@ -11396,7 +11856,7 @@
       <c r="N39" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O39" s="45" t="str">
+      <c r="O39" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en Kg de arándano por Cultivo</v>
       </c>
@@ -11407,7 +11867,9 @@
       <c r="R39" s="48">
         <v>1</v>
       </c>
-      <c r="S39" s="15"/>
+      <c r="S39" s="15" t="s">
+        <v>1005</v>
+      </c>
       <c r="V39" t="s">
         <v>949</v>
       </c>
@@ -11444,7 +11906,7 @@
       <c r="N40" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O40" s="45" t="str">
+      <c r="O40" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD de arándano por Cultivo</v>
       </c>
@@ -11455,7 +11917,9 @@
       <c r="R40" s="48">
         <v>1</v>
       </c>
-      <c r="S40" s="15"/>
+      <c r="S40" s="15" t="s">
+        <v>1006</v>
+      </c>
       <c r="V40" t="s">
         <v>949</v>
       </c>
@@ -11492,7 +11956,7 @@
       <c r="N41" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O41" s="45" t="str">
+      <c r="O41" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de arándano por Cultivo</v>
       </c>
@@ -11503,7 +11967,9 @@
       <c r="R41" s="48">
         <v>1</v>
       </c>
-      <c r="S41" s="15"/>
+      <c r="S41" s="15" t="s">
+        <v>1007</v>
+      </c>
       <c r="V41" t="s">
         <v>949</v>
       </c>
@@ -11540,7 +12006,7 @@
       <c r="N42" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O42" s="45" t="str">
+      <c r="O42" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en Kg de berries por Cultivo</v>
       </c>
@@ -11551,7 +12017,9 @@
       <c r="R42" s="48">
         <v>7</v>
       </c>
-      <c r="S42" s="15"/>
+      <c r="S42" s="15" t="s">
+        <v>1008</v>
+      </c>
       <c r="V42" t="s">
         <v>949</v>
       </c>
@@ -11588,7 +12056,7 @@
       <c r="N43" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O43" s="45" t="str">
+      <c r="O43" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD de berries por Cultivo</v>
       </c>
@@ -11599,7 +12067,9 @@
       <c r="R43" s="48">
         <v>7</v>
       </c>
-      <c r="S43" s="15"/>
+      <c r="S43" s="15" t="s">
+        <v>1009</v>
+      </c>
       <c r="V43" t="s">
         <v>949</v>
       </c>
@@ -11636,7 +12106,7 @@
       <c r="N44" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O44" s="45" t="str">
+      <c r="O44" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de berries por Cultivo</v>
       </c>
@@ -11647,7 +12117,9 @@
       <c r="R44" s="48">
         <v>7</v>
       </c>
-      <c r="S44" s="15"/>
+      <c r="S44" s="15" t="s">
+        <v>1010</v>
+      </c>
       <c r="V44" t="s">
         <v>949</v>
       </c>
@@ -11684,7 +12156,7 @@
       <c r="N45" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O45" s="45" t="str">
+      <c r="O45" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -11695,7 +12167,9 @@
       <c r="R45" s="48">
         <v>7</v>
       </c>
-      <c r="S45" s="15"/>
+      <c r="S45" s="15" t="s">
+        <v>1011</v>
+      </c>
       <c r="V45" t="s">
         <v>949</v>
       </c>
@@ -11732,7 +12206,7 @@
       <c r="N46" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O46" s="45" t="str">
+      <c r="O46" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en USD de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -11743,7 +12217,9 @@
       <c r="R46" s="48">
         <v>7</v>
       </c>
-      <c r="S46" s="15"/>
+      <c r="S46" s="15" t="s">
+        <v>1012</v>
+      </c>
       <c r="V46" t="s">
         <v>949</v>
       </c>
@@ -11780,7 +12256,7 @@
       <c r="N47" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O47" s="45" t="str">
+      <c r="O47" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -11791,7 +12267,9 @@
       <c r="R47" s="48">
         <v>7</v>
       </c>
-      <c r="S47" s="15"/>
+      <c r="S47" s="15" t="s">
+        <v>1013</v>
+      </c>
       <c r="V47" t="s">
         <v>949</v>
       </c>
@@ -11828,7 +12306,7 @@
       <c r="N48" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O48" s="45" t="str">
+      <c r="O48" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en Kg de Berries por Cultivo y Procesamiento</v>
       </c>
@@ -11839,7 +12317,9 @@
       <c r="R48" s="48">
         <v>7</v>
       </c>
-      <c r="S48" s="15"/>
+      <c r="S48" s="15" t="s">
+        <v>1014</v>
+      </c>
       <c r="V48" t="s">
         <v>949</v>
       </c>
@@ -11876,7 +12356,7 @@
       <c r="N49" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O49" s="45" t="str">
+      <c r="O49" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en USD de Berries por Cultivo y Procesamiento</v>
       </c>
@@ -11887,7 +12367,9 @@
       <c r="R49" s="48">
         <v>7</v>
       </c>
-      <c r="S49" s="15"/>
+      <c r="S49" s="15" t="s">
+        <v>1015</v>
+      </c>
       <c r="V49" t="s">
         <v>949</v>
       </c>
@@ -11924,7 +12406,7 @@
       <c r="N50" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O50" s="45" t="str">
+      <c r="O50" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de Berries por Cultivo y Procesamiento</v>
       </c>
@@ -11935,7 +12417,9 @@
       <c r="R50" s="48">
         <v>7</v>
       </c>
-      <c r="S50" s="15"/>
+      <c r="S50" s="15" t="s">
+        <v>1016</v>
+      </c>
       <c r="V50" t="s">
         <v>949</v>
       </c>
@@ -11972,7 +12456,7 @@
       <c r="N51" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O51" s="45" t="str">
+      <c r="O51" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en Kg de Berries por Cultivo y País de Destino</v>
       </c>
@@ -11983,7 +12467,9 @@
       <c r="R51" s="48">
         <v>7</v>
       </c>
-      <c r="S51" s="15"/>
+      <c r="S51" s="15" t="s">
+        <v>1017</v>
+      </c>
       <c r="V51" t="s">
         <v>949</v>
       </c>
@@ -12020,7 +12506,7 @@
       <c r="N52" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O52" s="45" t="str">
+      <c r="O52" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en USD de Berries por Cultivo y País de Destino</v>
       </c>
@@ -12031,7 +12517,9 @@
       <c r="R52" s="48">
         <v>7</v>
       </c>
-      <c r="S52" s="15"/>
+      <c r="S52" s="15" t="s">
+        <v>1018</v>
+      </c>
       <c r="V52" t="s">
         <v>949</v>
       </c>
@@ -12068,7 +12556,7 @@
       <c r="N53" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O53" s="45" t="str">
+      <c r="O53" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de Berries por Cultivo y País de Destino</v>
       </c>
@@ -12079,7 +12567,9 @@
       <c r="R53" s="48">
         <v>7</v>
       </c>
-      <c r="S53" s="15"/>
+      <c r="S53" s="15" t="s">
+        <v>1019</v>
+      </c>
       <c r="V53" t="s">
         <v>949</v>
       </c>
@@ -12113,7 +12603,7 @@
       <c r="N54" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O54" s="45" t="str">
+      <c r="O54" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en Kg de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -12124,7 +12614,9 @@
       <c r="R54" s="48">
         <v>110</v>
       </c>
-      <c r="S54" s="15"/>
+      <c r="S54" s="15" t="s">
+        <v>1020</v>
+      </c>
       <c r="V54" t="s">
         <v>949</v>
       </c>
@@ -12158,7 +12650,7 @@
       <c r="N55" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O55" s="45" t="str">
+      <c r="O55" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -12169,7 +12661,9 @@
       <c r="R55" s="48">
         <v>110</v>
       </c>
-      <c r="S55" s="15"/>
+      <c r="S55" s="15" t="s">
+        <v>1021</v>
+      </c>
       <c r="V55" t="s">
         <v>949</v>
       </c>
@@ -12203,7 +12697,7 @@
       <c r="N56" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O56" s="45" t="str">
+      <c r="O56" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -12214,6 +12708,9 @@
       <c r="R56" s="48">
         <v>110</v>
       </c>
+      <c r="S56" s="15" t="s">
+        <v>1022</v>
+      </c>
       <c r="V56" t="s">
         <v>949</v>
       </c>
@@ -12247,7 +12744,7 @@
       <c r="N57" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O57" s="45" t="str">
+      <c r="O57" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en Kg de arándano por Año</v>
       </c>
@@ -12258,7 +12755,9 @@
       <c r="R57" s="48">
         <v>110</v>
       </c>
-      <c r="S57" s="15"/>
+      <c r="S57" s="15" t="s">
+        <v>1023</v>
+      </c>
       <c r="V57" t="s">
         <v>949</v>
       </c>
@@ -12292,7 +12791,7 @@
       <c r="N58" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O58" s="45" t="str">
+      <c r="O58" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD de arándano por Año</v>
       </c>
@@ -12303,7 +12802,9 @@
       <c r="R58" s="48">
         <v>110</v>
       </c>
-      <c r="S58" s="15"/>
+      <c r="S58" s="15" t="s">
+        <v>1024</v>
+      </c>
       <c r="V58" t="s">
         <v>949</v>
       </c>
@@ -12337,7 +12838,7 @@
       <c r="N59" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O59" s="45" t="str">
+      <c r="O59" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de arándano por Año</v>
       </c>
@@ -12348,7 +12849,9 @@
       <c r="R59" s="48">
         <v>110</v>
       </c>
-      <c r="S59" s="15"/>
+      <c r="S59" s="15" t="s">
+        <v>1025</v>
+      </c>
       <c r="V59" t="s">
         <v>949</v>
       </c>
@@ -12382,7 +12885,7 @@
       <c r="N60" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O60" s="45" t="str">
+      <c r="O60" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en Kg de arándano por Procesamiento</v>
       </c>
@@ -12393,6 +12896,9 @@
       <c r="R60" s="48">
         <v>110</v>
       </c>
+      <c r="S60" s="15" t="s">
+        <v>1026</v>
+      </c>
       <c r="V60" t="s">
         <v>949</v>
       </c>
@@ -12426,7 +12932,7 @@
       <c r="N61" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O61" s="45" t="str">
+      <c r="O61" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD de arándano por Procesamiento</v>
       </c>
@@ -12437,6 +12943,9 @@
       <c r="R61" s="48">
         <v>110</v>
       </c>
+      <c r="S61" s="15" t="s">
+        <v>1027</v>
+      </c>
       <c r="V61" t="s">
         <v>949</v>
       </c>
@@ -12470,7 +12979,7 @@
       <c r="N62" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O62" s="45" t="str">
+      <c r="O62" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de arándano por Procesamiento</v>
       </c>
@@ -12481,6 +12990,9 @@
       <c r="R62" s="48">
         <v>110</v>
       </c>
+      <c r="S62" s="15" t="s">
+        <v>1028</v>
+      </c>
       <c r="V62" t="s">
         <v>949</v>
       </c>
@@ -12514,7 +13026,7 @@
       <c r="N63" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O63" s="45" t="str">
+      <c r="O63" s="79" t="str">
         <f>"Variación mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en Kg de arándano por País de destino</v>
       </c>
@@ -12525,6 +13037,9 @@
       <c r="R63" s="48">
         <v>110</v>
       </c>
+      <c r="S63" s="15" t="s">
+        <v>1029</v>
+      </c>
       <c r="V63" t="s">
         <v>949</v>
       </c>
@@ -12558,7 +13073,7 @@
       <c r="N64" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O64" s="45" t="str">
+      <c r="O64" s="80" t="str">
         <f>"Variación mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD de arándano por País de destino</v>
       </c>
@@ -12569,6 +13084,9 @@
       <c r="R64" s="48">
         <v>110</v>
       </c>
+      <c r="S64" s="15" t="s">
+        <v>1030</v>
+      </c>
       <c r="V64" t="s">
         <v>949</v>
       </c>
@@ -12602,7 +13120,7 @@
       <c r="N65" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O65" s="57" t="str">
+      <c r="O65" s="81" t="str">
         <f>"Variación mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Variación mensual de Exportaciones en USD/Kg de arándano por País de destino</v>
       </c>
@@ -12613,7 +13131,9 @@
       <c r="R65" s="60">
         <v>110</v>
       </c>
-      <c r="S65" s="15"/>
+      <c r="S65" s="15" t="s">
+        <v>1031</v>
+      </c>
       <c r="V65" t="s">
         <v>949</v>
       </c>
@@ -12647,7 +13167,7 @@
       <c r="N66" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O66" s="45" t="str">
+      <c r="O66" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en Kg de arándano por Cultivo</v>
       </c>
@@ -12658,6 +13178,9 @@
       <c r="R66" s="48">
         <v>1</v>
       </c>
+      <c r="S66" t="s">
+        <v>1032</v>
+      </c>
       <c r="V66" t="s">
         <v>949</v>
       </c>
@@ -12691,7 +13214,7 @@
       <c r="N67" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O67" s="45" t="str">
+      <c r="O67" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD de arándano por Cultivo</v>
       </c>
@@ -12702,7 +13225,9 @@
       <c r="R67" s="48">
         <v>1</v>
       </c>
-      <c r="S67" s="15"/>
+      <c r="S67" t="s">
+        <v>1032</v>
+      </c>
       <c r="V67" t="s">
         <v>949</v>
       </c>
@@ -12736,7 +13261,7 @@
       <c r="N68" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O68" s="45" t="str">
+      <c r="O68" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD/Kg de arándano por Cultivo</v>
       </c>
@@ -12747,6 +13272,9 @@
       <c r="R68" s="48">
         <v>1</v>
       </c>
+      <c r="S68" t="s">
+        <v>1032</v>
+      </c>
       <c r="V68" t="s">
         <v>949</v>
       </c>
@@ -12768,8 +13296,8 @@
       <c r="J69" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K69" s="41" t="s">
-        <v>10</v>
+      <c r="K69" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L69" s="42" t="s">
         <v>70</v>
@@ -12780,7 +13308,7 @@
       <c r="N69" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O69" s="45" t="str">
+      <c r="O69" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en Kg de berries por Cultivo</v>
       </c>
@@ -12791,6 +13319,10 @@
       <c r="R69" s="48">
         <v>7</v>
       </c>
+      <c r="S69" s="15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="T69" s="82"/>
       <c r="V69" t="s">
         <v>949</v>
       </c>
@@ -12812,8 +13344,8 @@
       <c r="J70" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K70" s="41" t="s">
-        <v>10</v>
+      <c r="K70" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L70" s="42" t="s">
         <v>70</v>
@@ -12824,7 +13356,7 @@
       <c r="N70" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O70" s="45" t="str">
+      <c r="O70" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD de berries por Cultivo</v>
       </c>
@@ -12835,7 +13367,9 @@
       <c r="R70" s="48">
         <v>7</v>
       </c>
-      <c r="S70" s="15"/>
+      <c r="S70" s="15" t="s">
+        <v>1035</v>
+      </c>
       <c r="V70" t="s">
         <v>949</v>
       </c>
@@ -12857,8 +13391,8 @@
       <c r="J71" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K71" s="41" t="s">
-        <v>10</v>
+      <c r="K71" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L71" s="42" t="s">
         <v>70</v>
@@ -12869,7 +13403,7 @@
       <c r="N71" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O71" s="45" t="str">
+      <c r="O71" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD/Kg de berries por Cultivo</v>
       </c>
@@ -12880,6 +13414,9 @@
       <c r="R71" s="48">
         <v>7</v>
       </c>
+      <c r="S71" s="15" t="s">
+        <v>1036</v>
+      </c>
       <c r="V71" t="s">
         <v>949</v>
       </c>
@@ -12902,7 +13439,7 @@
         <v>4</v>
       </c>
       <c r="K72" s="41" t="s">
-        <v>177</v>
+        <v>1037</v>
       </c>
       <c r="L72" s="42" t="s">
         <v>70</v>
@@ -12913,9 +13450,9 @@
       <c r="N72" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O72" s="45" t="str">
+      <c r="O72" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual de Exportaciones en Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
+        <v>Comparativo mensual de Exportaciones en Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico) - CULTIVO</v>
       </c>
       <c r="P72" s="46"/>
       <c r="Q72" s="47">
@@ -12924,6 +13461,9 @@
       <c r="R72" s="48">
         <v>7</v>
       </c>
+      <c r="S72" s="15" t="s">
+        <v>1038</v>
+      </c>
       <c r="V72" t="s">
         <v>949</v>
       </c>
@@ -12946,7 +13486,7 @@
         <v>4</v>
       </c>
       <c r="K73" s="41" t="s">
-        <v>177</v>
+        <v>1037</v>
       </c>
       <c r="L73" s="42" t="s">
         <v>70</v>
@@ -12957,9 +13497,9 @@
       <c r="N73" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O73" s="45" t="str">
+      <c r="O73" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual de Exportaciones en USD de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
+        <v>Comparativo mensual de Exportaciones en USD de Berries por Cultivo y Tipo (Orgánico/No orgánico) - CULTIVO</v>
       </c>
       <c r="P73" s="46"/>
       <c r="Q73" s="47">
@@ -12968,6 +13508,9 @@
       <c r="R73" s="48">
         <v>7</v>
       </c>
+      <c r="S73" s="15" t="s">
+        <v>1039</v>
+      </c>
       <c r="V73" t="s">
         <v>949</v>
       </c>
@@ -12990,7 +13533,7 @@
         <v>4</v>
       </c>
       <c r="K74" s="41" t="s">
-        <v>177</v>
+        <v>1037</v>
       </c>
       <c r="L74" s="42" t="s">
         <v>70</v>
@@ -13001,9 +13544,9 @@
       <c r="N74" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O74" s="45" t="str">
+      <c r="O74" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual de Exportaciones en USD/Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
+        <v>Comparativo mensual de Exportaciones en USD/Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico) - CULTIVO</v>
       </c>
       <c r="P74" s="46"/>
       <c r="Q74" s="47">
@@ -13012,6 +13555,9 @@
       <c r="R74" s="48">
         <v>7</v>
       </c>
+      <c r="S74" s="15" t="s">
+        <v>1040</v>
+      </c>
       <c r="V74" t="s">
         <v>949</v>
       </c>
@@ -13034,7 +13580,7 @@
         <v>4</v>
       </c>
       <c r="K75" s="41" t="s">
-        <v>181</v>
+        <v>1044</v>
       </c>
       <c r="L75" s="42" t="s">
         <v>70</v>
@@ -13045,9 +13591,9 @@
       <c r="N75" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O75" s="45" t="str">
+      <c r="O75" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual de Exportaciones en Kg de Berries por Cultivo y Procesamiento</v>
+        <v>Comparativo mensual de Exportaciones en Kg de Berries por Cultivo y Procesamiento - CULTIVO</v>
       </c>
       <c r="P75" s="46"/>
       <c r="Q75" s="47">
@@ -13056,6 +13602,9 @@
       <c r="R75" s="48">
         <v>7</v>
       </c>
+      <c r="S75" s="15" t="s">
+        <v>1041</v>
+      </c>
       <c r="V75" t="s">
         <v>949</v>
       </c>
@@ -13078,7 +13627,7 @@
         <v>4</v>
       </c>
       <c r="K76" s="41" t="s">
-        <v>181</v>
+        <v>1044</v>
       </c>
       <c r="L76" s="42" t="s">
         <v>70</v>
@@ -13089,9 +13638,9 @@
       <c r="N76" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O76" s="45" t="str">
+      <c r="O76" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual de Exportaciones en USD de Berries por Cultivo y Procesamiento</v>
+        <v>Comparativo mensual de Exportaciones en USD de Berries por Cultivo y Procesamiento - CULTIVO</v>
       </c>
       <c r="P76" s="46"/>
       <c r="Q76" s="47">
@@ -13100,6 +13649,9 @@
       <c r="R76" s="48">
         <v>7</v>
       </c>
+      <c r="S76" s="15" t="s">
+        <v>1042</v>
+      </c>
       <c r="V76" t="s">
         <v>949</v>
       </c>
@@ -13122,7 +13674,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="41" t="s">
-        <v>181</v>
+        <v>1044</v>
       </c>
       <c r="L77" s="42" t="s">
         <v>70</v>
@@ -13133,9 +13685,9 @@
       <c r="N77" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O77" s="45" t="str">
+      <c r="O77" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual de Exportaciones en USD/Kg de Berries por Cultivo y Procesamiento</v>
+        <v>Comparativo mensual de Exportaciones en USD/Kg de Berries por Cultivo y Procesamiento - CULTIVO</v>
       </c>
       <c r="P77" s="46"/>
       <c r="Q77" s="47">
@@ -13144,6 +13696,9 @@
       <c r="R77" s="48">
         <v>7</v>
       </c>
+      <c r="S77" s="15" t="s">
+        <v>1043</v>
+      </c>
       <c r="V77" t="s">
         <v>949</v>
       </c>
@@ -13177,7 +13732,7 @@
       <c r="N78" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O78" s="45" t="str">
+      <c r="O78" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Comparativo mensual de Exportaciones en Kg de Berries por Cultivo y País de Destino</v>
       </c>
@@ -13188,6 +13743,9 @@
       <c r="R78" s="48">
         <v>7</v>
       </c>
+      <c r="S78" s="15" t="s">
+        <v>1045</v>
+      </c>
       <c r="V78" t="s">
         <v>949</v>
       </c>
@@ -13221,7 +13779,7 @@
       <c r="N79" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O79" s="45" t="str">
+      <c r="O79" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Comparativo mensual de Exportaciones en USD de Berries por Cultivo y País de Destino</v>
       </c>
@@ -13232,6 +13790,9 @@
       <c r="R79" s="48">
         <v>7</v>
       </c>
+      <c r="S79" s="15" t="s">
+        <v>1046</v>
+      </c>
       <c r="V79" t="s">
         <v>949</v>
       </c>
@@ -13265,7 +13826,7 @@
       <c r="N80" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O80" s="45" t="str">
+      <c r="O80" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Comparativo mensual de Exportaciones en USD/Kg de Berries por Cultivo y País de Destino</v>
       </c>
@@ -13276,6 +13837,9 @@
       <c r="R80" s="48">
         <v>7</v>
       </c>
+      <c r="S80" s="15" t="s">
+        <v>1047</v>
+      </c>
       <c r="V80" t="s">
         <v>949</v>
       </c>
@@ -13288,7 +13852,6 @@
         <v>141</v>
       </c>
       <c r="H81" s="9">
-        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="I81" s="40" t="s">
@@ -13309,7 +13872,7 @@
       <c r="N81" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O81" s="45" t="str">
+      <c r="O81" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en Kg de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -13320,6 +13883,9 @@
       <c r="R81" s="48">
         <v>110</v>
       </c>
+      <c r="S81" s="15" t="s">
+        <v>1048</v>
+      </c>
       <c r="V81" t="s">
         <v>949</v>
       </c>
@@ -13353,7 +13919,7 @@
       <c r="N82" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O82" s="45" t="str">
+      <c r="O82" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -13364,6 +13930,9 @@
       <c r="R82" s="48">
         <v>110</v>
       </c>
+      <c r="S82" s="15" t="s">
+        <v>1049</v>
+      </c>
       <c r="V82" t="s">
         <v>949</v>
       </c>
@@ -13397,7 +13966,7 @@
       <c r="N83" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O83" s="45" t="str">
+      <c r="O83" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD/Kg de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -13408,6 +13977,9 @@
       <c r="R83" s="48">
         <v>110</v>
       </c>
+      <c r="S83" s="15" t="s">
+        <v>1050</v>
+      </c>
       <c r="V83" t="s">
         <v>949</v>
       </c>
@@ -13441,7 +14013,7 @@
       <c r="N84" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O84" s="45" t="str">
+      <c r="O84" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en Kg de arándano por Año</v>
       </c>
@@ -13452,6 +14024,9 @@
       <c r="R84" s="48">
         <v>110</v>
       </c>
+      <c r="S84" t="s">
+        <v>1051</v>
+      </c>
       <c r="V84" t="s">
         <v>949</v>
       </c>
@@ -13485,7 +14060,7 @@
       <c r="N85" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O85" s="45" t="str">
+      <c r="O85" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD de arándano por Año</v>
       </c>
@@ -13496,6 +14071,9 @@
       <c r="R85" s="48">
         <v>110</v>
       </c>
+      <c r="S85" t="s">
+        <v>1052</v>
+      </c>
       <c r="V85" t="s">
         <v>949</v>
       </c>
@@ -13529,7 +14107,7 @@
       <c r="N86" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O86" s="45" t="str">
+      <c r="O86" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD/Kg de arándano por Año</v>
       </c>
@@ -13540,6 +14118,9 @@
       <c r="R86" s="48">
         <v>110</v>
       </c>
+      <c r="S86" t="s">
+        <v>1053</v>
+      </c>
       <c r="V86" t="s">
         <v>949</v>
       </c>
@@ -13552,7 +14133,6 @@
         <v>147</v>
       </c>
       <c r="H87" s="9">
-        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="I87" s="40" t="s">
@@ -13573,7 +14153,7 @@
       <c r="N87" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O87" s="45" t="str">
+      <c r="O87" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en Kg de arándano por Procesamiento</v>
       </c>
@@ -13584,6 +14164,9 @@
       <c r="R87" s="48">
         <v>110</v>
       </c>
+      <c r="S87" s="15" t="s">
+        <v>1054</v>
+      </c>
       <c r="V87" t="s">
         <v>949</v>
       </c>
@@ -13617,7 +14200,7 @@
       <c r="N88" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O88" s="45" t="str">
+      <c r="O88" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD de arándano por Procesamiento</v>
       </c>
@@ -13628,6 +14211,9 @@
       <c r="R88" s="48">
         <v>110</v>
       </c>
+      <c r="S88" s="15" t="s">
+        <v>1055</v>
+      </c>
       <c r="V88" t="s">
         <v>949</v>
       </c>
@@ -13661,7 +14247,7 @@
       <c r="N89" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O89" s="45" t="str">
+      <c r="O89" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD/Kg de arándano por Procesamiento</v>
       </c>
@@ -13672,6 +14258,9 @@
       <c r="R89" s="48">
         <v>110</v>
       </c>
+      <c r="S89" s="15" t="s">
+        <v>1056</v>
+      </c>
       <c r="V89" t="s">
         <v>949</v>
       </c>
@@ -13705,7 +14294,7 @@
       <c r="N90" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O90" s="45" t="str">
+      <c r="O90" s="79" t="str">
         <f>"Comparativo mensual de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en Kg de arándano por País de destino</v>
       </c>
@@ -13716,6 +14305,9 @@
       <c r="R90" s="48">
         <v>110</v>
       </c>
+      <c r="S90" s="15" t="s">
+        <v>1057</v>
+      </c>
       <c r="V90" t="s">
         <v>949</v>
       </c>
@@ -13749,7 +14341,7 @@
       <c r="N91" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="O91" s="45" t="str">
+      <c r="O91" s="80" t="str">
         <f>"Comparativo mensual de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD de arándano por País de destino</v>
       </c>
@@ -13760,6 +14352,9 @@
       <c r="R91" s="48">
         <v>110</v>
       </c>
+      <c r="S91" s="15" t="s">
+        <v>1058</v>
+      </c>
       <c r="V91" t="s">
         <v>949</v>
       </c>
@@ -13793,7 +14388,7 @@
       <c r="N92" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="O92" s="57" t="str">
+      <c r="O92" s="81" t="str">
         <f>"Comparativo mensual de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual de Exportaciones en USD/Kg de arándano por País de destino</v>
       </c>
@@ -13804,6 +14399,9 @@
       <c r="R92" s="60">
         <v>110</v>
       </c>
+      <c r="S92" s="15" t="s">
+        <v>1059</v>
+      </c>
       <c r="V92" t="s">
         <v>949</v>
       </c>
@@ -13825,8 +14423,8 @@
       <c r="J93" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K93" s="41" t="s">
-        <v>10</v>
+      <c r="K93" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L93" s="42" t="s">
         <v>70</v>
@@ -13837,7 +14435,7 @@
       <c r="N93" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O93" s="45" t="str">
+      <c r="O93" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en Kg de arándano por Cultivo</v>
       </c>
@@ -13848,6 +14446,9 @@
       <c r="R93" s="48">
         <v>1</v>
       </c>
+      <c r="S93" s="15" t="s">
+        <v>1063</v>
+      </c>
       <c r="V93" t="s">
         <v>949</v>
       </c>
@@ -13869,8 +14470,8 @@
       <c r="J94" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K94" s="41" t="s">
-        <v>10</v>
+      <c r="K94" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L94" s="42" t="s">
         <v>70</v>
@@ -13881,7 +14482,7 @@
       <c r="N94" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O94" s="45" t="str">
+      <c r="O94" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD de arándano por Cultivo</v>
       </c>
@@ -13892,6 +14493,9 @@
       <c r="R94" s="48">
         <v>1</v>
       </c>
+      <c r="S94" s="15" t="s">
+        <v>1064</v>
+      </c>
       <c r="V94" t="s">
         <v>949</v>
       </c>
@@ -13913,8 +14517,8 @@
       <c r="J95" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K95" s="41" t="s">
-        <v>10</v>
+      <c r="K95" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L95" s="42" t="s">
         <v>70</v>
@@ -13925,7 +14529,7 @@
       <c r="N95" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O95" s="45" t="str">
+      <c r="O95" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de arándano por Cultivo</v>
       </c>
@@ -13936,6 +14540,9 @@
       <c r="R95" s="48">
         <v>1</v>
       </c>
+      <c r="S95" s="15" t="s">
+        <v>1065</v>
+      </c>
       <c r="V95" t="s">
         <v>949</v>
       </c>
@@ -13957,8 +14564,8 @@
       <c r="J96" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K96" s="41" t="s">
-        <v>10</v>
+      <c r="K96" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L96" s="42" t="s">
         <v>70</v>
@@ -13969,7 +14576,7 @@
       <c r="N96" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O96" s="45" t="str">
+      <c r="O96" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en Kg de berries por Cultivo</v>
       </c>
@@ -13980,6 +14587,9 @@
       <c r="R96" s="48">
         <v>7</v>
       </c>
+      <c r="S96" s="15" t="s">
+        <v>1060</v>
+      </c>
       <c r="V96" t="s">
         <v>949</v>
       </c>
@@ -14001,8 +14611,8 @@
       <c r="J97" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K97" s="41" t="s">
-        <v>10</v>
+      <c r="K97" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L97" s="42" t="s">
         <v>70</v>
@@ -14013,7 +14623,7 @@
       <c r="N97" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O97" s="45" t="str">
+      <c r="O97" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD de berries por Cultivo</v>
       </c>
@@ -14024,6 +14634,9 @@
       <c r="R97" s="48">
         <v>7</v>
       </c>
+      <c r="S97" s="15" t="s">
+        <v>1061</v>
+      </c>
       <c r="V97" t="s">
         <v>949</v>
       </c>
@@ -14045,8 +14658,8 @@
       <c r="J98" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K98" s="41" t="s">
-        <v>10</v>
+      <c r="K98" s="83" t="s">
+        <v>1033</v>
       </c>
       <c r="L98" s="42" t="s">
         <v>70</v>
@@ -14057,7 +14670,7 @@
       <c r="N98" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O98" s="45" t="str">
+      <c r="O98" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de berries por Cultivo</v>
       </c>
@@ -14068,6 +14681,9 @@
       <c r="R98" s="48">
         <v>7</v>
       </c>
+      <c r="S98" s="15" t="s">
+        <v>1062</v>
+      </c>
       <c r="V98" t="s">
         <v>949</v>
       </c>
@@ -14090,7 +14706,7 @@
         <v>4</v>
       </c>
       <c r="K99" s="41" t="s">
-        <v>177</v>
+        <v>1037</v>
       </c>
       <c r="L99" s="42" t="s">
         <v>70</v>
@@ -14101,9 +14717,9 @@
       <c r="N99" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O99" s="45" t="str">
+      <c r="O99" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual últimos dos años de Exportaciones en Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
+        <v>Comparativo mensual últimos dos años de Exportaciones en Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico) - CULTIVO</v>
       </c>
       <c r="P99" s="46"/>
       <c r="Q99" s="47">
@@ -14112,6 +14728,9 @@
       <c r="R99" s="48">
         <v>7</v>
       </c>
+      <c r="S99" s="15" t="s">
+        <v>1066</v>
+      </c>
       <c r="V99" t="s">
         <v>949</v>
       </c>
@@ -14134,7 +14753,7 @@
         <v>4</v>
       </c>
       <c r="K100" s="41" t="s">
-        <v>177</v>
+        <v>1037</v>
       </c>
       <c r="L100" s="42" t="s">
         <v>70</v>
@@ -14145,9 +14764,9 @@
       <c r="N100" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O100" s="45" t="str">
+      <c r="O100" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual últimos dos años de Exportaciones en USD de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
+        <v>Comparativo mensual últimos dos años de Exportaciones en USD de Berries por Cultivo y Tipo (Orgánico/No orgánico) - CULTIVO</v>
       </c>
       <c r="P100" s="46"/>
       <c r="Q100" s="47">
@@ -14156,6 +14775,9 @@
       <c r="R100" s="48">
         <v>7</v>
       </c>
+      <c r="S100" s="15" t="s">
+        <v>1067</v>
+      </c>
       <c r="V100" t="s">
         <v>949</v>
       </c>
@@ -14178,7 +14800,7 @@
         <v>4</v>
       </c>
       <c r="K101" s="41" t="s">
-        <v>177</v>
+        <v>1037</v>
       </c>
       <c r="L101" s="42" t="s">
         <v>70</v>
@@ -14189,9 +14811,9 @@
       <c r="N101" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O101" s="45" t="str">
+      <c r="O101" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico)</v>
+        <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de Berries por Cultivo y Tipo (Orgánico/No orgánico) - CULTIVO</v>
       </c>
       <c r="P101" s="46"/>
       <c r="Q101" s="47">
@@ -14200,6 +14822,9 @@
       <c r="R101" s="48">
         <v>7</v>
       </c>
+      <c r="S101" s="15" t="s">
+        <v>1068</v>
+      </c>
       <c r="V101" t="s">
         <v>949</v>
       </c>
@@ -14222,7 +14847,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="41" t="s">
-        <v>181</v>
+        <v>1044</v>
       </c>
       <c r="L102" s="42" t="s">
         <v>70</v>
@@ -14233,9 +14858,9 @@
       <c r="N102" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O102" s="45" t="str">
+      <c r="O102" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual últimos dos años de Exportaciones en Kg de Berries por Cultivo y Procesamiento</v>
+        <v>Comparativo mensual últimos dos años de Exportaciones en Kg de Berries por Cultivo y Procesamiento - CULTIVO</v>
       </c>
       <c r="P102" s="46"/>
       <c r="Q102" s="47">
@@ -14244,6 +14869,9 @@
       <c r="R102" s="48">
         <v>7</v>
       </c>
+      <c r="S102" s="15" t="s">
+        <v>1069</v>
+      </c>
       <c r="V102" t="s">
         <v>949</v>
       </c>
@@ -14266,7 +14894,7 @@
         <v>4</v>
       </c>
       <c r="K103" s="41" t="s">
-        <v>181</v>
+        <v>1044</v>
       </c>
       <c r="L103" s="42" t="s">
         <v>70</v>
@@ -14277,9 +14905,9 @@
       <c r="N103" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O103" s="45" t="str">
+      <c r="O103" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual últimos dos años de Exportaciones en USD de Berries por Cultivo y Procesamiento</v>
+        <v>Comparativo mensual últimos dos años de Exportaciones en USD de Berries por Cultivo y Procesamiento - CULTIVO</v>
       </c>
       <c r="P103" s="46"/>
       <c r="Q103" s="47">
@@ -14288,6 +14916,9 @@
       <c r="R103" s="48">
         <v>7</v>
       </c>
+      <c r="S103" s="15" t="s">
+        <v>1070</v>
+      </c>
       <c r="V103" t="s">
         <v>949</v>
       </c>
@@ -14310,7 +14941,7 @@
         <v>4</v>
       </c>
       <c r="K104" s="41" t="s">
-        <v>181</v>
+        <v>1044</v>
       </c>
       <c r="L104" s="42" t="s">
         <v>70</v>
@@ -14321,9 +14952,9 @@
       <c r="N104" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O104" s="45" t="str">
+      <c r="O104" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
-        <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de Berries por Cultivo y Procesamiento</v>
+        <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de Berries por Cultivo y Procesamiento - CULTIVO</v>
       </c>
       <c r="P104" s="46"/>
       <c r="Q104" s="47">
@@ -14332,6 +14963,9 @@
       <c r="R104" s="48">
         <v>7</v>
       </c>
+      <c r="S104" s="15" t="s">
+        <v>1071</v>
+      </c>
       <c r="V104" t="s">
         <v>949</v>
       </c>
@@ -14365,7 +14999,7 @@
       <c r="N105" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O105" s="45" t="str">
+      <c r="O105" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en Kg de Berries por Cultivo y País de Destino</v>
       </c>
@@ -14376,6 +15010,9 @@
       <c r="R105" s="48">
         <v>7</v>
       </c>
+      <c r="S105" s="15" t="s">
+        <v>1072</v>
+      </c>
       <c r="V105" t="s">
         <v>949</v>
       </c>
@@ -14409,7 +15046,7 @@
       <c r="N106" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O106" s="45" t="str">
+      <c r="O106" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD de Berries por Cultivo y País de Destino</v>
       </c>
@@ -14420,6 +15057,9 @@
       <c r="R106" s="48">
         <v>7</v>
       </c>
+      <c r="S106" s="15" t="s">
+        <v>1073</v>
+      </c>
       <c r="V106" t="s">
         <v>949</v>
       </c>
@@ -14453,7 +15093,7 @@
       <c r="N107" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O107" s="45" t="str">
+      <c r="O107" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de Berries por "&amp;Tabla1[[#This Row],[Variable]]&amp;" y "&amp;Tabla1[[#This Row],[Filtro Int]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de Berries por Cultivo y País de Destino</v>
       </c>
@@ -14464,6 +15104,9 @@
       <c r="R107" s="48">
         <v>7</v>
       </c>
+      <c r="S107" s="15" t="s">
+        <v>1074</v>
+      </c>
       <c r="V107" t="s">
         <v>949</v>
       </c>
@@ -14497,7 +15140,7 @@
       <c r="N108" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O108" s="45" t="str">
+      <c r="O108" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en Kg de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -14508,6 +15151,9 @@
       <c r="R108" s="48">
         <v>110</v>
       </c>
+      <c r="S108" s="15" t="s">
+        <v>1075</v>
+      </c>
       <c r="V108" t="s">
         <v>949</v>
       </c>
@@ -14541,7 +15187,7 @@
       <c r="N109" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O109" s="45" t="str">
+      <c r="O109" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -14552,6 +15198,9 @@
       <c r="R109" s="48">
         <v>110</v>
       </c>
+      <c r="S109" s="15" t="s">
+        <v>1076</v>
+      </c>
       <c r="V109" t="s">
         <v>949</v>
       </c>
@@ -14585,7 +15234,7 @@
       <c r="N110" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O110" s="45" t="str">
+      <c r="O110" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de arándano por Tipo (Orgánico/No orgánico)</v>
       </c>
@@ -14596,6 +15245,9 @@
       <c r="R110" s="48">
         <v>110</v>
       </c>
+      <c r="S110" s="15" t="s">
+        <v>1077</v>
+      </c>
       <c r="V110" t="s">
         <v>949</v>
       </c>
@@ -14629,7 +15281,7 @@
       <c r="N111" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O111" s="45" t="str">
+      <c r="O111" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en Kg de arándano por Año</v>
       </c>
@@ -14640,6 +15292,9 @@
       <c r="R111" s="48">
         <v>110</v>
       </c>
+      <c r="S111" s="15" t="s">
+        <v>1078</v>
+      </c>
       <c r="V111" t="s">
         <v>949</v>
       </c>
@@ -14673,7 +15328,7 @@
       <c r="N112" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O112" s="45" t="str">
+      <c r="O112" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD de arándano por Año</v>
       </c>
@@ -14684,6 +15339,9 @@
       <c r="R112" s="48">
         <v>110</v>
       </c>
+      <c r="S112" s="15" t="s">
+        <v>1079</v>
+      </c>
       <c r="V112" t="s">
         <v>949</v>
       </c>
@@ -14717,7 +15375,7 @@
       <c r="N113" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O113" s="45" t="str">
+      <c r="O113" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de arándano por Año</v>
       </c>
@@ -14728,6 +15386,9 @@
       <c r="R113" s="48">
         <v>110</v>
       </c>
+      <c r="S113" s="15" t="s">
+        <v>1080</v>
+      </c>
       <c r="V113" t="s">
         <v>949</v>
       </c>
@@ -14761,7 +15422,7 @@
       <c r="N114" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O114" s="45" t="str">
+      <c r="O114" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en Kg de arándano por Procesamiento</v>
       </c>
@@ -14772,6 +15433,9 @@
       <c r="R114" s="48">
         <v>110</v>
       </c>
+      <c r="S114" s="15" t="s">
+        <v>1081</v>
+      </c>
       <c r="V114" t="s">
         <v>949</v>
       </c>
@@ -14805,7 +15469,7 @@
       <c r="N115" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O115" s="45" t="str">
+      <c r="O115" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD de arándano por Procesamiento</v>
       </c>
@@ -14816,6 +15480,9 @@
       <c r="R115" s="48">
         <v>110</v>
       </c>
+      <c r="S115" s="15" t="s">
+        <v>1082</v>
+      </c>
       <c r="V115" t="s">
         <v>949</v>
       </c>
@@ -14849,7 +15516,7 @@
       <c r="N116" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O116" s="45" t="str">
+      <c r="O116" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de arándano por Procesamiento</v>
       </c>
@@ -14860,6 +15527,9 @@
       <c r="R116" s="48">
         <v>110</v>
       </c>
+      <c r="S116" s="15" t="s">
+        <v>1083</v>
+      </c>
       <c r="V116" t="s">
         <v>949</v>
       </c>
@@ -14893,7 +15563,7 @@
       <c r="N117" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O117" s="45" t="str">
+      <c r="O117" s="79" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B2&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en Kg de arándano por País de destino</v>
       </c>
@@ -14904,6 +15574,9 @@
       <c r="R117" s="48">
         <v>110</v>
       </c>
+      <c r="S117" s="15" t="s">
+        <v>1084</v>
+      </c>
       <c r="V117" t="s">
         <v>949</v>
       </c>
@@ -14937,7 +15610,7 @@
       <c r="N118" s="44" t="s">
         <v>935</v>
       </c>
-      <c r="O118" s="45" t="str">
+      <c r="O118" s="80" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B3&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD de arándano por País de destino</v>
       </c>
@@ -14948,6 +15621,9 @@
       <c r="R118" s="48">
         <v>110</v>
       </c>
+      <c r="S118" s="15" t="s">
+        <v>1085</v>
+      </c>
       <c r="V118" t="s">
         <v>949</v>
       </c>
@@ -14981,7 +15657,7 @@
       <c r="N119" s="56" t="s">
         <v>935</v>
       </c>
-      <c r="O119" s="57" t="str">
+      <c r="O119" s="81" t="str">
         <f>"Comparativo mensual últimos dos años de "&amp;B4&amp;""&amp;" de arándano por "&amp;Tabla1[[#This Row],[Variable]]</f>
         <v>Comparativo mensual últimos dos años de Exportaciones en USD/Kg de arándano por País de destino</v>
       </c>
@@ -14992,6 +15668,9 @@
       <c r="R119" s="60">
         <v>110</v>
       </c>
+      <c r="S119" s="15" t="s">
+        <v>1086</v>
+      </c>
       <c r="V119" t="s">
         <v>949</v>
       </c>
@@ -15036,6 +15715,9 @@
       <c r="R120" s="48">
         <v>1</v>
       </c>
+      <c r="S120" s="15" t="s">
+        <v>1087</v>
+      </c>
       <c r="V120" t="s">
         <v>949</v>
       </c>
@@ -15080,6 +15762,9 @@
       <c r="R121" s="48">
         <v>1</v>
       </c>
+      <c r="S121" s="15" t="s">
+        <v>1088</v>
+      </c>
       <c r="V121" t="s">
         <v>949</v>
       </c>
@@ -15124,6 +15809,9 @@
       <c r="R122" s="48">
         <v>1</v>
       </c>
+      <c r="S122" s="15" t="s">
+        <v>1089</v>
+      </c>
       <c r="V122" t="s">
         <v>949</v>
       </c>
@@ -15158,8 +15846,8 @@
         <v>950</v>
       </c>
       <c r="O123" s="45" t="str">
-        <f>"Valumen mensual de "&amp;B2&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
-        <v>Valumen mensual de Exportaciones en Kg de berries por Cultivo</v>
+        <f>"Volumen mensual de "&amp;B2&amp;""&amp;" de berries por "&amp;Tabla1[[#This Row],[Variable]]</f>
+        <v>Volumen mensual de Exportaciones en Kg de berries por Cultivo</v>
       </c>
       <c r="P123" s="46"/>
       <c r="Q123" s="47">
@@ -15168,6 +15856,9 @@
       <c r="R123" s="48">
         <v>7</v>
       </c>
+      <c r="S123" s="15" t="s">
+        <v>1090</v>
+      </c>
       <c r="V123" t="s">
         <v>949</v>
       </c>
@@ -15212,6 +15903,9 @@
       <c r="R124" s="48">
         <v>7</v>
       </c>
+      <c r="S124" s="15" t="s">
+        <v>1091</v>
+      </c>
       <c r="V124" t="s">
         <v>949</v>
       </c>
@@ -15256,6 +15950,9 @@
       <c r="R125" s="48">
         <v>7</v>
       </c>
+      <c r="S125" s="15" t="s">
+        <v>1092</v>
+      </c>
       <c r="V125" t="s">
         <v>949</v>
       </c>
@@ -15300,6 +15997,9 @@
       <c r="R126" s="48">
         <v>7</v>
       </c>
+      <c r="S126" s="15" t="s">
+        <v>1093</v>
+      </c>
       <c r="V126" t="s">
         <v>949</v>
       </c>
@@ -15344,6 +16044,9 @@
       <c r="R127" s="48">
         <v>7</v>
       </c>
+      <c r="S127" s="15" t="s">
+        <v>1094</v>
+      </c>
       <c r="V127" t="s">
         <v>949</v>
       </c>
@@ -15388,6 +16091,9 @@
       <c r="R128" s="48">
         <v>7</v>
       </c>
+      <c r="S128" s="15" t="s">
+        <v>1095</v>
+      </c>
       <c r="V128" t="s">
         <v>949</v>
       </c>
@@ -15432,6 +16138,9 @@
       <c r="R129" s="48">
         <v>7</v>
       </c>
+      <c r="S129" s="15" t="s">
+        <v>1096</v>
+      </c>
       <c r="V129" t="s">
         <v>949</v>
       </c>
@@ -15476,6 +16185,9 @@
       <c r="R130" s="48">
         <v>7</v>
       </c>
+      <c r="S130" s="15" t="s">
+        <v>1097</v>
+      </c>
       <c r="V130" t="s">
         <v>949</v>
       </c>
@@ -15520,6 +16232,9 @@
       <c r="R131" s="48">
         <v>7</v>
       </c>
+      <c r="S131" s="15" t="s">
+        <v>1098</v>
+      </c>
       <c r="V131" t="s">
         <v>949</v>
       </c>
@@ -15564,6 +16279,9 @@
       <c r="R132" s="48">
         <v>110</v>
       </c>
+      <c r="S132" s="15" t="s">
+        <v>1099</v>
+      </c>
       <c r="V132" t="s">
         <v>949</v>
       </c>
@@ -15608,6 +16326,9 @@
       <c r="R133" s="48">
         <v>110</v>
       </c>
+      <c r="S133" s="15" t="s">
+        <v>1100</v>
+      </c>
       <c r="V133" t="s">
         <v>949</v>
       </c>
@@ -15652,6 +16373,9 @@
       <c r="R134" s="48">
         <v>110</v>
       </c>
+      <c r="S134" s="15" t="s">
+        <v>1101</v>
+      </c>
       <c r="V134" t="s">
         <v>949</v>
       </c>
@@ -15696,6 +16420,9 @@
       <c r="R135" s="48">
         <v>110</v>
       </c>
+      <c r="S135" s="15" t="s">
+        <v>1102</v>
+      </c>
       <c r="V135" t="s">
         <v>949</v>
       </c>
@@ -15740,6 +16467,9 @@
       <c r="R136" s="48">
         <v>110</v>
       </c>
+      <c r="S136" s="15" t="s">
+        <v>1103</v>
+      </c>
       <c r="V136" t="s">
         <v>949</v>
       </c>
@@ -15784,6 +16514,9 @@
       <c r="R137" s="48">
         <v>110</v>
       </c>
+      <c r="S137" s="15" t="s">
+        <v>1104</v>
+      </c>
       <c r="V137" t="s">
         <v>949</v>
       </c>
@@ -15828,6 +16561,9 @@
       <c r="R138" s="48">
         <v>110</v>
       </c>
+      <c r="S138" s="15" t="s">
+        <v>1105</v>
+      </c>
       <c r="V138" t="s">
         <v>949</v>
       </c>
@@ -15872,6 +16608,9 @@
       <c r="R139" s="76">
         <v>110</v>
       </c>
+      <c r="S139" s="15" t="s">
+        <v>1106</v>
+      </c>
       <c r="V139" t="s">
         <v>949</v>
       </c>
@@ -15916,7 +16655,9 @@
       <c r="R140" s="60">
         <v>110</v>
       </c>
-      <c r="S140" s="77"/>
+      <c r="S140" s="84" t="s">
+        <v>1107</v>
+      </c>
       <c r="T140" s="77"/>
       <c r="U140" s="77"/>
       <c r="V140" t="s">
@@ -15940,8 +16681,8 @@
       <c r="J141" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K141" s="41" t="s">
-        <v>10</v>
+      <c r="K141" s="83" t="s">
+        <v>1108</v>
       </c>
       <c r="L141" s="42" t="s">
         <v>625</v>
@@ -15963,7 +16704,9 @@
       <c r="R141" s="48">
         <v>6</v>
       </c>
-      <c r="S141" s="77"/>
+      <c r="S141" s="84" t="s">
+        <v>1109</v>
+      </c>
       <c r="T141" s="77"/>
       <c r="U141" s="77"/>
       <c r="V141" t="s">
@@ -15987,8 +16730,8 @@
       <c r="J142" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K142" s="41" t="s">
-        <v>10</v>
+      <c r="K142" s="83" t="s">
+        <v>1108</v>
       </c>
       <c r="L142" s="42" t="s">
         <v>625</v>
@@ -16010,7 +16753,9 @@
       <c r="R142" s="48">
         <v>6</v>
       </c>
-      <c r="S142" s="77"/>
+      <c r="S142" s="84" t="s">
+        <v>1110</v>
+      </c>
       <c r="T142" s="77"/>
       <c r="U142" s="77"/>
       <c r="V142" t="s">
@@ -16034,8 +16779,8 @@
       <c r="J143" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K143" s="41" t="s">
-        <v>10</v>
+      <c r="K143" s="83" t="s">
+        <v>1108</v>
       </c>
       <c r="L143" s="42" t="s">
         <v>625</v>
@@ -16057,7 +16802,9 @@
       <c r="R143" s="48">
         <v>6</v>
       </c>
-      <c r="S143" s="77"/>
+      <c r="S143" s="84" t="s">
+        <v>1111</v>
+      </c>
       <c r="T143" s="77"/>
       <c r="U143" s="77"/>
       <c r="V143" t="s">
@@ -16082,7 +16829,7 @@
         <v>4</v>
       </c>
       <c r="K144" s="41" t="s">
-        <v>177</v>
+        <v>1115</v>
       </c>
       <c r="L144" s="42" t="s">
         <v>70</v>
@@ -16104,7 +16851,9 @@
       <c r="R144" s="48">
         <v>6</v>
       </c>
-      <c r="S144" s="77"/>
+      <c r="S144" s="84" t="s">
+        <v>1112</v>
+      </c>
       <c r="T144" s="77"/>
       <c r="U144" s="77"/>
       <c r="V144" t="s">
@@ -16129,7 +16878,7 @@
         <v>4</v>
       </c>
       <c r="K145" s="41" t="s">
-        <v>177</v>
+        <v>1115</v>
       </c>
       <c r="L145" s="42" t="s">
         <v>70</v>
@@ -16151,7 +16900,9 @@
       <c r="R145" s="48">
         <v>6</v>
       </c>
-      <c r="S145" s="77"/>
+      <c r="S145" s="84" t="s">
+        <v>1113</v>
+      </c>
       <c r="T145" s="77"/>
       <c r="U145" s="77"/>
       <c r="V145" t="s">
@@ -16175,8 +16926,8 @@
       <c r="J146" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="K146" s="52" t="s">
-        <v>177</v>
+      <c r="K146" s="41" t="s">
+        <v>1115</v>
       </c>
       <c r="L146" s="54" t="s">
         <v>70</v>
@@ -16198,7 +16949,9 @@
       <c r="R146" s="60">
         <v>6</v>
       </c>
-      <c r="S146" s="77"/>
+      <c r="S146" s="84" t="s">
+        <v>1114</v>
+      </c>
       <c r="T146" s="77"/>
       <c r="U146" s="77"/>
       <c r="V146" t="s">
@@ -16220,17 +16973,101 @@
     <hyperlink ref="S26" r:id="rId6" xr:uid="{3731900F-7698-49B4-9CF2-1349DC3386CE}"/>
     <hyperlink ref="S15" r:id="rId7" xr:uid="{FC0D2906-AD12-4496-8DA2-0CD563667CB0}"/>
     <hyperlink ref="S18" r:id="rId8" xr:uid="{4A164919-AFBB-4724-9E06-8C5D16EA7A0A}"/>
+    <hyperlink ref="S41" r:id="rId9" xr:uid="{AA7B7BAC-DCFB-4DA5-94A2-4C9FC74BF06A}"/>
+    <hyperlink ref="S42" r:id="rId10" xr:uid="{140FB9D6-6B08-42DA-B195-59300C1C563E}"/>
+    <hyperlink ref="S43" r:id="rId11" xr:uid="{3DFEF9F9-E090-4384-B5A1-1DE34C6186E3}"/>
+    <hyperlink ref="S44" r:id="rId12" xr:uid="{DC2EC6ED-264A-40F6-BFD0-F4831959A076}"/>
+    <hyperlink ref="S56" r:id="rId13" xr:uid="{792B04A5-6447-4B8F-A5D7-C4785C67BC58}"/>
+    <hyperlink ref="S60" r:id="rId14" xr:uid="{F8FBB1A4-9405-400A-B596-D30F2255D5D4}"/>
+    <hyperlink ref="S61" r:id="rId15" xr:uid="{F14DAA16-2206-4E01-931F-F916100E93B9}"/>
+    <hyperlink ref="S62" r:id="rId16" xr:uid="{E654B389-7159-47A9-AD0E-69D711425CD0}"/>
+    <hyperlink ref="S63" r:id="rId17" xr:uid="{6F59DD78-E79A-41B4-AB26-E44238A08374}"/>
+    <hyperlink ref="S64" r:id="rId18" xr:uid="{01A3A8EF-4269-4592-AB2E-F0865F943963}"/>
+    <hyperlink ref="S69" r:id="rId19" xr:uid="{EB8B6851-B573-445B-B9B1-A4A3E14F5ACE}"/>
+    <hyperlink ref="S71" r:id="rId20" xr:uid="{35ED0CD8-C178-4A56-A845-D60410487C26}"/>
+    <hyperlink ref="S72" r:id="rId21" xr:uid="{6D68FEFC-89B1-49F4-B080-8DEE40EB6BAD}"/>
+    <hyperlink ref="S73" r:id="rId22" xr:uid="{EFEF7BF8-F3A8-4E76-BAEE-1C924ECC1583}"/>
+    <hyperlink ref="S74" r:id="rId23" xr:uid="{24BFAE0A-121E-4340-BDAF-3B6DE7894C63}"/>
+    <hyperlink ref="S75" r:id="rId24" xr:uid="{63383D14-F069-4298-94B1-F323656A4DB3}"/>
+    <hyperlink ref="S76" r:id="rId25" xr:uid="{AB4DC9DD-97C4-467E-B108-B7DFF5EDDF89}"/>
+    <hyperlink ref="S77" r:id="rId26" xr:uid="{46FCB078-4927-4DCF-AC31-6773F776F0B1}"/>
+    <hyperlink ref="S78" r:id="rId27" xr:uid="{FB3305E0-20B0-404E-8041-515BD855B1CE}"/>
+    <hyperlink ref="S79" r:id="rId28" xr:uid="{85081A43-D38E-44DE-83E4-B0548171F455}"/>
+    <hyperlink ref="S80" r:id="rId29" xr:uid="{2F893D31-2121-4598-A030-63B7580692A6}"/>
+    <hyperlink ref="S81" r:id="rId30" xr:uid="{AC3324F9-A513-41D0-9C98-0D752138EAE7}"/>
+    <hyperlink ref="S82" r:id="rId31" xr:uid="{1A2E31E9-DC0E-4690-86F4-9AD35C37DAF4}"/>
+    <hyperlink ref="S83" r:id="rId32" xr:uid="{F4BF8B80-F618-4568-ADC9-665354456562}"/>
+    <hyperlink ref="S87" r:id="rId33" xr:uid="{64C2D2AA-043B-41E1-B941-66F5E35EB472}"/>
+    <hyperlink ref="S88" r:id="rId34" xr:uid="{A8FF3DB2-7CDD-48F8-B497-7FC262DB0897}"/>
+    <hyperlink ref="S89" r:id="rId35" xr:uid="{F060C1D8-2D37-4559-A090-0C89CA6B9DF2}"/>
+    <hyperlink ref="S90" r:id="rId36" xr:uid="{B9909DC0-7527-40B5-A7FD-370458CB49D2}"/>
+    <hyperlink ref="S91" r:id="rId37" xr:uid="{7F6402D0-31DC-45AA-846D-21A2A0752916}"/>
+    <hyperlink ref="S92" r:id="rId38" xr:uid="{13462F16-1488-45BA-8C73-C23C5E4B96F9}"/>
+    <hyperlink ref="S96" r:id="rId39" xr:uid="{CC173AA4-2485-4E6C-8FAC-05E724843750}"/>
+    <hyperlink ref="S97" r:id="rId40" xr:uid="{D77F183B-826B-47CE-9F8D-D4A442C4A62F}"/>
+    <hyperlink ref="S98" r:id="rId41" xr:uid="{6832C325-DB67-47B0-BE1D-BDBEE7AE9A42}"/>
+    <hyperlink ref="S93" r:id="rId42" xr:uid="{1B39369E-1872-4C6A-8498-2E0F7F256D75}"/>
+    <hyperlink ref="S94" r:id="rId43" xr:uid="{71167866-4317-448D-8400-297AF98DF054}"/>
+    <hyperlink ref="S95" r:id="rId44" xr:uid="{1C451EA8-5F9F-41B2-99DD-DD43C0837A28}"/>
+    <hyperlink ref="S99" r:id="rId45" xr:uid="{BEB17728-5EEE-43B5-862F-357E686EAB6C}"/>
+    <hyperlink ref="S100" r:id="rId46" xr:uid="{C81138A4-FC34-4A30-8555-0D306A6F4FDE}"/>
+    <hyperlink ref="S101" r:id="rId47" xr:uid="{ACEEF2FE-C5EE-4E42-BC45-803BBE3640A0}"/>
+    <hyperlink ref="S102" r:id="rId48" xr:uid="{16A1AC9E-C55A-43C0-8702-3B1463E1E182}"/>
+    <hyperlink ref="S103" r:id="rId49" xr:uid="{66F3999E-2C4E-45F0-84F1-C0A0C1FA0F41}"/>
+    <hyperlink ref="S104" r:id="rId50" xr:uid="{DE4EC9CA-CCCF-437C-9C14-9ADCE52C25AE}"/>
+    <hyperlink ref="S105" r:id="rId51" xr:uid="{F9C80E50-857D-414E-8128-0288648A4071}"/>
+    <hyperlink ref="S106" r:id="rId52" xr:uid="{EAB3202E-7796-4841-9381-95249F0D1EA6}"/>
+    <hyperlink ref="S107" r:id="rId53" xr:uid="{16F76CE1-73AF-4DDE-9F59-CA10AC66FD2F}"/>
+    <hyperlink ref="S108" r:id="rId54" xr:uid="{A86E9668-0DBD-4F35-B121-AAC399602CD4}"/>
+    <hyperlink ref="S109" r:id="rId55" xr:uid="{299A979C-728F-489A-B427-45E1D4126A74}"/>
+    <hyperlink ref="S110" r:id="rId56" xr:uid="{8B6136DE-FA74-467D-B591-3545881D3F8F}"/>
+    <hyperlink ref="S111" r:id="rId57" xr:uid="{B81FF752-4431-4FB6-91EE-8F25A0A61A2C}"/>
+    <hyperlink ref="S112" r:id="rId58" xr:uid="{93F9F7EE-6518-4C4F-8031-CF6D71FAC12E}"/>
+    <hyperlink ref="S113" r:id="rId59" xr:uid="{97C58B6B-52AE-4380-A2D7-B34D1FA22CAD}"/>
+    <hyperlink ref="S114" r:id="rId60" xr:uid="{16E1A70A-42BC-4837-B7A2-E2ACFA6AB478}"/>
+    <hyperlink ref="S115" r:id="rId61" xr:uid="{1D1BBC63-D3CB-4A62-8258-44AA977EDFAC}"/>
+    <hyperlink ref="S116" r:id="rId62" xr:uid="{A91D4270-26A0-491A-BC75-2105EBC23C84}"/>
+    <hyperlink ref="S117" r:id="rId63" xr:uid="{E58DAE36-E035-4655-98F4-BD13FAAC7C62}"/>
+    <hyperlink ref="S118" r:id="rId64" xr:uid="{D5A5EDCD-2377-4495-B527-A5A1217FD73B}"/>
+    <hyperlink ref="S119" r:id="rId65" xr:uid="{B763B26F-ADAC-4A6A-8382-0B41A33126B9}"/>
+    <hyperlink ref="S120" r:id="rId66" xr:uid="{57A0C9FC-9E39-4E31-B801-A3B171535849}"/>
+    <hyperlink ref="S121" r:id="rId67" xr:uid="{F3532A5E-DB89-43D9-9657-D74D31572088}"/>
+    <hyperlink ref="S122" r:id="rId68" xr:uid="{6EFB6527-6DB3-4DAE-AB03-5FD774F30FA4}"/>
+    <hyperlink ref="S123" r:id="rId69" xr:uid="{CA68C421-6FAA-416D-84F9-B6A715B7C1FB}"/>
+    <hyperlink ref="S124" r:id="rId70" xr:uid="{BB0B9557-DD15-4C5C-AFC0-AFAD352C618D}"/>
+    <hyperlink ref="S125" r:id="rId71" xr:uid="{5CE5E8E8-C7AB-4665-A26A-D8C4F813C518}"/>
+    <hyperlink ref="S126" r:id="rId72" xr:uid="{E7E0C75A-99EA-4D04-872E-F6A372364887}"/>
+    <hyperlink ref="S127" r:id="rId73" xr:uid="{3B63280D-47D0-4964-A201-4D3DDF3B781A}"/>
+    <hyperlink ref="S128" r:id="rId74" xr:uid="{9C3106CD-9551-493E-9FD0-5622405EBD7F}"/>
+    <hyperlink ref="S129" r:id="rId75" xr:uid="{E9EC645F-D7A9-4EC5-8098-9C00C0BB84E0}"/>
+    <hyperlink ref="S130" r:id="rId76" xr:uid="{4698A89A-0ABD-41B5-9567-3886DE5AED1A}"/>
+    <hyperlink ref="S131" r:id="rId77" xr:uid="{C98EFA8F-A2F1-4B80-A8A2-99E386884066}"/>
+    <hyperlink ref="S132" r:id="rId78" xr:uid="{23BA8AC4-E407-42BA-9CC3-8E442722FC0D}"/>
+    <hyperlink ref="S133" r:id="rId79" xr:uid="{634DFEC8-686C-4233-8084-C3C121FBE6C1}"/>
+    <hyperlink ref="S134" r:id="rId80" xr:uid="{4BD79C5A-203C-49A9-AA0B-CB0716F100C0}"/>
+    <hyperlink ref="S135" r:id="rId81" xr:uid="{116AA143-3E0B-403D-BB21-E29D1863DFD8}"/>
+    <hyperlink ref="S136" r:id="rId82" xr:uid="{4FFAF665-A0A0-4A41-993B-4A1EFDEDD97E}"/>
+    <hyperlink ref="S137" r:id="rId83" xr:uid="{F4704E8A-C839-47A0-826D-FC7333C85D5E}"/>
+    <hyperlink ref="S138" r:id="rId84" xr:uid="{44966BDA-5CB8-4532-815A-14421F816E81}"/>
+    <hyperlink ref="S139" r:id="rId85" xr:uid="{66B69BC6-B24E-4659-B4CE-D01873ECA6F3}"/>
+    <hyperlink ref="S140" r:id="rId86" xr:uid="{C13B0C14-B7AD-48A3-B06D-065C6864720F}"/>
+    <hyperlink ref="S141" r:id="rId87" xr:uid="{71669452-46C4-4ECB-B5F6-CA5082932F79}"/>
+    <hyperlink ref="S142" r:id="rId88" xr:uid="{34138367-7577-4209-9F42-7E33BB078CA5}"/>
+    <hyperlink ref="S143" r:id="rId89" xr:uid="{3066703E-F79D-4DE8-B9DB-D5F75CE81835}"/>
+    <hyperlink ref="S144" r:id="rId90" xr:uid="{C337587C-5076-4B3A-A6D2-FD9CC472AF41}"/>
+    <hyperlink ref="S145" r:id="rId91" xr:uid="{EDDD3F10-5107-4371-8738-CEEB3327608B}"/>
+    <hyperlink ref="S146" r:id="rId92" xr:uid="{5214C2B2-64D2-4F18-8DA9-4C5264C299D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
-  <drawing r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId93"/>
+  <drawing r:id="rId94"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId95"/>
   </tableParts>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId12"/>
+        <x14:slicer r:id="rId96"/>
       </x14:slicerList>
     </ext>
   </extLst>
@@ -22670,7 +23507,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C111">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>